<commit_message>
docs: use case diagram, use case description 수정 - 자전거 대여소 리스트 조회, 대여소 상세정보 조회 use case 분리
</commit_message>
<xml_diff>
--- a/강지완/usecase_description_강지완.xlsx
+++ b/강지완/usecase_description_강지완.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SE_Team2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SE_Team2\강지완\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591CC6AC-F9FD-4D56-B3FC-F62ED6AF8645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F75BB82-C58B-4365-A828-3DDCE10D3752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9A1A4C-40C9-46E0-9101-937DFF5848E6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9A1A4C-40C9-46E0-9101-937DFF5848E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>로그인</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,26 +122,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3. 관리자가 특정 대여소를 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4. 시스템은 선택된 대여소의 상세정보 화면을 표시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. 관리자가 상세 정보 화면에서 삭제 버튼 선택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6. 시스템은 선택된 대여소의 삭제 여부를 확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7. 관리자가 삭제를 확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>8. 시스템은 해당 대여소를 DB에서 삭제하고 리스트를 갱신</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -167,6 +147,42 @@
   </si>
   <si>
     <t>4. 로그인 페이지 또는 홈 화면으로 리디렉션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 관리자가 특정 대여소를 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자전거 대여소 상세정보 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 시스템은 자전거 대여소 리스트 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 시스템은 선택된 대여소의 상세정보 화면을 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 관리자가 자전거 대여소 리스트에서 삭제 버튼 선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 시스템은 선택된 대여소의 삭제 여부를 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. 관리자가 삭제를 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. 시스템은 해당 대여소를 DB에서 삭제하고 리스트를 갱신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. 시스템은 삭제 확인 메시지를 출력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -216,7 +232,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -300,13 +316,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -316,56 +345,77 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -707,295 +757,365 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32EF711-E41E-4776-BBB7-C6C14271EF27}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="60.625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="60.625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="60.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="60.625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="11" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="11" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="17" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="11" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="18"/>
     </row>
     <row r="11" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="12" t="s">
+      <c r="A13" s="15"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="12" t="s">
-        <v>31</v>
+      <c r="A14" s="15"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-    </row>
+      <c r="A15" s="16"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>3</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="13"/>
     </row>
     <row r="18" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="8" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="11" t="s">
+      <c r="A20" s="15"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="15"/>
+      <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="11" t="s">
+      <c r="A23" s="15"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="11" t="s">
+      <c r="A24" s="15"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="11" t="s">
-        <v>30</v>
+      <c r="A25" s="16"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
     </row>
     <row r="27" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>4</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="9" t="s">
+      <c r="A28" s="19"/>
+      <c r="B28" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="20"/>
+      <c r="B29" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="12" t="s">
+      <c r="A30" s="20"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
-      <c r="B31" s="9" t="s">
+      <c r="A31" s="20"/>
+      <c r="B31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="20"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="20"/>
+      <c r="B33" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="20"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="20"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="20"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="12"/>
-    </row>
-    <row r="32" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="6"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6"/>
-      <c r="B33" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="12"/>
-    </row>
-    <row r="34" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="12" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="21"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
-      <c r="B35" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="12"/>
-    </row>
-    <row r="36" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="12" t="s">
+    <row r="39" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>5</v>
+      </c>
+      <c r="B39" s="13" t="s">
         <v>29</v>
       </c>
+      <c r="C39" s="13"/>
+    </row>
+    <row r="40" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="14"/>
+      <c r="B40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="15"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="15"/>
+      <c r="B42" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="26"/>
+    </row>
+    <row r="43" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="16"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="23"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="28"/>
+    </row>
+    <row r="45" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="23"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="28"/>
+    </row>
+    <row r="46" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="23"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="28"/>
+    </row>
+    <row r="47" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="23"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="28"/>
+    </row>
+    <row r="48" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="23"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="28"/>
+    </row>
+    <row r="49" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="23"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
+    </row>
+    <row r="50" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="23"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A40:A43"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A28:A37"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B17:C17"/>

</xml_diff>